<commit_message>
Implemenation of industry historical load by Uche
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\TPC-DI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDMA\Data warehouses\TPC_DI\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C6C859-7716-4ADD-966C-C5C825895E69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD894841-866B-418D-97EA-CBFEE0C19324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical load" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Table</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AM34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,9 @@
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="AM4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Industry and datetime done
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\TPC-DI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDMA\Data warehouses\TPC_DI\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F51A80-0249-4C93-A405-AEE8963B2C30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E125F254-7D35-4914-AAFD-7C1F811B2A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical load" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Table</t>
   </si>
@@ -213,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -222,6 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +578,7 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -595,7 +596,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -604,14 +605,16 @@
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="AM3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">

</xml_diff>

<commit_message>
Statustype, taxrate, tradetype done.
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDMA\Data warehouses\TPC_DI\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E125F254-7D35-4914-AAFD-7C1F811B2A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D71F19-5B8A-4FAD-9B27-F9DB6FE31222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Table</t>
   </si>
@@ -540,7 +540,7 @@
   <dimension ref="A1:AM34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,10 +599,10 @@
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -631,31 +631,37 @@
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">

</xml_diff>

<commit_message>
DimAccount and DimCustomer incremental updates
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fun\Desktop\TPC-DI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\tmp 2\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F4B939-9607-4331-98E9-958FB322256F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E90B416-2CBA-4AED-82EE-6B39E24F9697}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical load" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="51">
   <si>
     <t>Table</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>FactMarketHistory</t>
+  </si>
+  <si>
+    <t>DimCustomer_incemental</t>
+  </si>
+  <si>
+    <t>DimAccount_incemental</t>
+  </si>
+  <si>
+    <t>Customer.txt</t>
+  </si>
+  <si>
+    <t>Account.txt</t>
   </si>
 </sst>
 </file>
@@ -581,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +602,7 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -847,14 +859,26 @@
       </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="6"/>
+      <c r="E21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>

</xml_diff>

<commit_message>
DimTrade incremental ready. Datatype change for DimTrade Init
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\tmp\TPC-DI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\tmp2\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148DC729-3E53-482C-9003-0FB74A4FD29F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325BFA5F-582A-4ADF-8358-6A344633E2D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="53">
   <si>
     <t>Table</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E23" sqref="E23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,11 +889,11 @@
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prospect increamental updates done
</commit_message>
<xml_diff>
--- a/Implementation plan.xlsx
+++ b/Implementation plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayadi\OneDrive\Documents\GitHub\TPC-DI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fun\Desktop\tpdi\TPC-DI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AF81FA-2AC9-45E3-8E66-43D6DE0A7993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31ED327-6A45-48FB-808D-A96C031A093F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1020" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical load" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E24" sqref="E24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,11 +904,11 @@
       </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>